<commit_message>
adicionando atributos em excelservice
</commit_message>
<xml_diff>
--- a/src/main/resources/files/Modelo_Praca.xlsx
+++ b/src/main/resources/files/Modelo_Praca.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t xml:space="preserve">Nome completo</t>
   </si>
@@ -55,13 +55,25 @@
     <t xml:space="preserve">MASCULINO</t>
   </si>
   <si>
-    <t xml:space="preserve">“”</t>
-  </si>
-  <si>
     <t xml:space="preserve">1º ano do Ensino Médio</t>
   </si>
   <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U</t>
+  </si>
+  <si>
     <t xml:space="preserve">Medicina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maria José</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FEMININO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Direito</t>
   </si>
 </sst>
 </file>
@@ -71,7 +83,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -122,6 +134,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -171,7 +189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -192,6 +210,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -209,10 +231,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y3"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -286,23 +308,23 @@
       <c r="C2" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>11</v>
+      <c r="D2" s="0" t="n">
+        <v>5426</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1456212435</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="H2" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -320,7 +342,35 @@
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>555</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>1456212435</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>